<commit_message>
third organization commit 2/2024
</commit_message>
<xml_diff>
--- a/Dictionary.xlsx
+++ b/Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\R Projects\Species_interactions_mediate_SGD_effects_coral_physiology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D9AC0E-8DFB-4E0E-BEE3-AE4A0D79A7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B3C745-21BF-4841-B397-AFD8D883A9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="2" xr2:uid="{B84DB3B6-3B42-44E8-BFD8-7CA6897F3F30}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="453">
   <si>
     <t>File Name</t>
   </si>
@@ -824,7 +824,580 @@
     <t>physiology_analysis</t>
   </si>
   <si>
-    <t>Analysis markdown normalizing CC to SA</t>
+    <t>ID for respirometry trial group</t>
+  </si>
+  <si>
+    <t>Date of respirometry trial</t>
+  </si>
+  <si>
+    <t>Raw O2 File name</t>
+  </si>
+  <si>
+    <t>Light or dark O2 measurements</t>
+  </si>
+  <si>
+    <t>Varari</t>
+  </si>
+  <si>
+    <t>BLANK Y/N for</t>
+  </si>
+  <si>
+    <t>Notes for the respirometry trial</t>
+  </si>
+  <si>
+    <t>Trial start time</t>
+  </si>
+  <si>
+    <t>Trial stop time</t>
+  </si>
+  <si>
+    <t>Volume of water in the respirometry chamber</t>
+  </si>
+  <si>
+    <t>Total surface area</t>
+  </si>
+  <si>
+    <t>Person who measured the coral fragment (Sabrina or Jamie)</t>
+  </si>
+  <si>
+    <t>Weight of the coral fragment before wax</t>
+  </si>
+  <si>
+    <t>Weight of the coral fragment after wax</t>
+  </si>
+  <si>
+    <t>Diameter of wooden dowel used for calibration curve</t>
+  </si>
+  <si>
+    <t>Height of wooden dowel used for calibration curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated surface area of wooden dowel </t>
+  </si>
+  <si>
+    <t>Weight of wooden dowel before wax</t>
+  </si>
+  <si>
+    <t>Weight of wooden dowel after wax</t>
+  </si>
+  <si>
+    <t>Weight of the wax</t>
+  </si>
+  <si>
+    <t>Dowel ID</t>
+  </si>
+  <si>
+    <t>Fragment type (pre-deployment physio or PR, PR curve, post-deployment)</t>
+  </si>
+  <si>
+    <t>Volume of filtered saltwater and coral tissue blastate of fragment</t>
+  </si>
+  <si>
+    <t>The total number of blastate tubes for each coral (used to track the tubes)</t>
+  </si>
+  <si>
+    <t>Notes for blastate</t>
+  </si>
+  <si>
+    <t>CT_xxx_Varari</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>Date  and time of CT log measurement</t>
+  </si>
+  <si>
+    <t>Temperature value from CT logger</t>
+  </si>
+  <si>
+    <t>Site CT Logger is located (Varari only used in this study)</t>
+  </si>
+  <si>
+    <t>Plate that the CT logger was at</t>
+  </si>
+  <si>
+    <t>Logger ID</t>
+  </si>
+  <si>
+    <t>ID for the CT logger</t>
+  </si>
+  <si>
+    <t>Date_launched</t>
+  </si>
+  <si>
+    <t>Date the CT logger was launched</t>
+  </si>
+  <si>
+    <t>Tiime_launched</t>
+  </si>
+  <si>
+    <t>Time the CT logger was launched</t>
+  </si>
+  <si>
+    <t>Date_retrieved</t>
+  </si>
+  <si>
+    <t>Date the CT logger was retrieved</t>
+  </si>
+  <si>
+    <t>Time_retrieved</t>
+  </si>
+  <si>
+    <t>Time the CT logger was retrieved</t>
+  </si>
+  <si>
+    <t>CT Logger notes</t>
+  </si>
+  <si>
+    <t>Date and time of CT log measurement</t>
+  </si>
+  <si>
+    <t>LoggerID</t>
+  </si>
+  <si>
+    <t>FullLoggerID</t>
+  </si>
+  <si>
+    <t>Full ID for the CT logger</t>
+  </si>
+  <si>
+    <t>TempInSitu</t>
+  </si>
+  <si>
+    <t>E_Cond</t>
+  </si>
+  <si>
+    <t>Conductivity value from CT logger</t>
+  </si>
+  <si>
+    <t>Salinity_psu</t>
+  </si>
+  <si>
+    <t>Salinity value from CT logger</t>
+  </si>
+  <si>
+    <t>Plate that the Turbinaria was collected from</t>
+  </si>
+  <si>
+    <t>Sample_Weight</t>
+  </si>
+  <si>
+    <t>Weight of the Turbinaria sample</t>
+  </si>
+  <si>
+    <t>N_ug</t>
+  </si>
+  <si>
+    <t>Nitrogen content in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>del15N</t>
+  </si>
+  <si>
+    <t>Del15N in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>C_ug</t>
+  </si>
+  <si>
+    <t>Carbon content in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>del13C</t>
+  </si>
+  <si>
+    <t>Del13C in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>N_percent</t>
+  </si>
+  <si>
+    <t>Percent nitrogen in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>C_percent</t>
+  </si>
+  <si>
+    <t>Percent carbon in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>C_N</t>
+  </si>
+  <si>
+    <t>Carbon to nitrogen ratio in Turbinaria sample</t>
+  </si>
+  <si>
+    <t>Plate that the coral was randomly assigned to</t>
+  </si>
+  <si>
+    <t>Plate_ID</t>
+  </si>
+  <si>
+    <t>ID of the plate</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Plate ID</t>
+  </si>
+  <si>
+    <t>Treatment (m, c, h, s)</t>
+  </si>
+  <si>
+    <t>Missing_central</t>
+  </si>
+  <si>
+    <t>The number of center corals missing (binary)</t>
+  </si>
+  <si>
+    <t>Missing_comp</t>
+  </si>
+  <si>
+    <t>The number of neighbor corals missing (0-4)</t>
+  </si>
+  <si>
+    <t>Notes on missing fragments</t>
+  </si>
+  <si>
+    <t>Top_Plate_ID</t>
+  </si>
+  <si>
+    <t>Bottom_Plate_ID</t>
+  </si>
+  <si>
+    <t>Jamie_Plate_ID</t>
+  </si>
+  <si>
+    <t>GPS_ID</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>CreationTime</t>
+  </si>
+  <si>
+    <t>Of the sandwiched plates for both projects, ID for the top plates (this project)</t>
+  </si>
+  <si>
+    <t>ID for the bottom plates (another project)</t>
+  </si>
+  <si>
+    <t>ID for the plates for this project</t>
+  </si>
+  <si>
+    <t>Name of the plate location in the GPS</t>
+  </si>
+  <si>
+    <t>Site (Varari was only used in this experiment)</t>
+  </si>
+  <si>
+    <t>Plate latitude</t>
+  </si>
+  <si>
+    <t>Plate longitude</t>
+  </si>
+  <si>
+    <t>Creation Time</t>
+  </si>
+  <si>
+    <t>Associated cow tag to the plate</t>
+  </si>
+  <si>
+    <t>SurfaceAreaInitial</t>
+  </si>
+  <si>
+    <t>Initial surface area of the coral fragment</t>
+  </si>
+  <si>
+    <t>NetPhotoInitial</t>
+  </si>
+  <si>
+    <t>Initial net photosynthesis of the coral donor colony</t>
+  </si>
+  <si>
+    <t>GrossPhotoInitial</t>
+  </si>
+  <si>
+    <t>Initial gross photosynthesis of the coral donor colony</t>
+  </si>
+  <si>
+    <t>RespirationInitial</t>
+  </si>
+  <si>
+    <t>Initial respiration of the coral donor colony</t>
+  </si>
+  <si>
+    <t>ID for the coral fragment</t>
+  </si>
+  <si>
+    <t>SurfaceAreaFinal</t>
+  </si>
+  <si>
+    <t>Final surface area of the coral fragment</t>
+  </si>
+  <si>
+    <t>NetPhotoFinal</t>
+  </si>
+  <si>
+    <t>GrossPhotoFinal</t>
+  </si>
+  <si>
+    <t>Final net photosynthesis of the coral fragment</t>
+  </si>
+  <si>
+    <t>Final gross photosynthesis of the coral fragment</t>
+  </si>
+  <si>
+    <t>RespirationFinal</t>
+  </si>
+  <si>
+    <t>Final respiration of the coral fragment</t>
+  </si>
+  <si>
+    <t>pc_change_GP</t>
+  </si>
+  <si>
+    <t>Percent change in gross photosynthesis</t>
+  </si>
+  <si>
+    <t>pc_change_NP</t>
+  </si>
+  <si>
+    <t>Percent change in net photosynthesis</t>
+  </si>
+  <si>
+    <t>pc_change_R</t>
+  </si>
+  <si>
+    <t>Percent change in respiration</t>
+  </si>
+  <si>
+    <t>ID of the coral fragment</t>
+  </si>
+  <si>
+    <t>Treatment (no neighbor (m), Dead skeletal (s), Conspecific (c), Heterospecific (h))</t>
+  </si>
+  <si>
+    <t>Response_measurement</t>
+  </si>
+  <si>
+    <t>Response measurement- chlorophyll content, endosymbiont density, net photosynthesis, gross photosynthesis, or respiration</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Initial value of the response measurement pre-deployment</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Final value of the response measurement post-deployment</t>
+  </si>
+  <si>
+    <t>ID of the fragment</t>
+  </si>
+  <si>
+    <t>Site (Varari)</t>
+  </si>
+  <si>
+    <t>Biogeochemical measurement</t>
+  </si>
+  <si>
+    <t>Predictor_measurement</t>
+  </si>
+  <si>
+    <t>Predictor_value</t>
+  </si>
+  <si>
+    <t>Biogeochemical value</t>
+  </si>
+  <si>
+    <t>Scaled biogeochemical value</t>
+  </si>
+  <si>
+    <t>minTemp</t>
+  </si>
+  <si>
+    <t>Minimum temperature</t>
+  </si>
+  <si>
+    <t>maxTemp</t>
+  </si>
+  <si>
+    <t>Maximum temperature</t>
+  </si>
+  <si>
+    <t>meanTemp</t>
+  </si>
+  <si>
+    <t>Mean temperature</t>
+  </si>
+  <si>
+    <t>rangeTemp</t>
+  </si>
+  <si>
+    <t>Range of temperature</t>
+  </si>
+  <si>
+    <t>Covariance of temperature</t>
+  </si>
+  <si>
+    <t>cvTemp</t>
+  </si>
+  <si>
+    <t>Site latitude</t>
+  </si>
+  <si>
+    <t>Site longitude</t>
+  </si>
+  <si>
+    <t>Date of measurement</t>
+  </si>
+  <si>
+    <t>Time of measurement</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Date and time of measurement</t>
+  </si>
+  <si>
+    <t>Tide</t>
+  </si>
+  <si>
+    <t>Tide (high or low)</t>
+  </si>
+  <si>
+    <t>Day_Night</t>
+  </si>
+  <si>
+    <t>Day or night</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>Salinity of sample</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Temperature of sample</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Total alkalinity of sample</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>pH of sample</t>
+  </si>
+  <si>
+    <t>Phosphate_umolL</t>
+  </si>
+  <si>
+    <t>Phosphate concentration of sample</t>
+  </si>
+  <si>
+    <t>Silicate_umolL</t>
+  </si>
+  <si>
+    <t>Silicate concentration of sample</t>
+  </si>
+  <si>
+    <t>NN_umolL</t>
+  </si>
+  <si>
+    <t>Nitrate + nitrite concentration of sample</t>
+  </si>
+  <si>
+    <t>Ammonia_umolL</t>
+  </si>
+  <si>
+    <t>Ammonia concentration of sample</t>
+  </si>
+  <si>
+    <t>min, means, max, and range of the measured biogeochemical variables</t>
+  </si>
+  <si>
+    <t>Raw value of biogeochemical measurement</t>
+  </si>
+  <si>
+    <t>Predictor_scaled</t>
+  </si>
+  <si>
+    <t>Scaled value of biogeochemical measurement</t>
+  </si>
+  <si>
+    <t>Min analysis- Analysis markdown normalizing CC to SA</t>
+  </si>
+  <si>
+    <t>Chlorophyll content</t>
+  </si>
+  <si>
+    <t>Endosymbiont density</t>
+  </si>
+  <si>
+    <t>Final photosynthesis and respiration</t>
+  </si>
+  <si>
+    <t>Initial photosynthesis and respiration</t>
+  </si>
+  <si>
+    <t>Combined photosynthesis and respiration</t>
+  </si>
+  <si>
+    <t>Surface area</t>
+  </si>
+  <si>
+    <t>Coral physiological response + biogeochemical measurements</t>
+  </si>
+  <si>
+    <t>Coral physiological responses (long)</t>
+  </si>
+  <si>
+    <t>CT measurements</t>
+  </si>
+  <si>
+    <t>Summary of CT measurements</t>
+  </si>
+  <si>
+    <t>Turbinaria sample measurements</t>
+  </si>
+  <si>
+    <t>Raw values of biogeochemical measurement summaries</t>
+  </si>
+  <si>
+    <t>Scaled values of biogeochemical measurement summaries</t>
+  </si>
+  <si>
+    <t>Raw data from Silibger repo of biogeochemical sampling</t>
+  </si>
+  <si>
+    <t>Summary data of biogeochemical measurements</t>
   </si>
 </sst>
 </file>
@@ -1184,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE711FF-9152-461F-BB3A-6765DB4F4886}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1861,7 +2434,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1869,7 +2442,7 @@
     <col min="1" max="1" width="19.64453125" customWidth="1"/>
     <col min="2" max="2" width="23.5859375" customWidth="1"/>
     <col min="3" max="3" width="33.29296875" customWidth="1"/>
-    <col min="4" max="4" width="19.64453125" customWidth="1"/>
+    <col min="4" max="4" width="44.3515625" customWidth="1"/>
     <col min="5" max="5" width="28.52734375" customWidth="1"/>
     <col min="6" max="6" width="19.64453125" customWidth="1"/>
   </cols>
@@ -1909,6 +2482,9 @@
       <c r="C4" t="s">
         <v>56</v>
       </c>
+      <c r="D4" t="s">
+        <v>438</v>
+      </c>
       <c r="E4" t="s">
         <v>52</v>
       </c>
@@ -1926,6 +2502,9 @@
       <c r="C5" t="s">
         <v>83</v>
       </c>
+      <c r="D5" t="s">
+        <v>439</v>
+      </c>
       <c r="E5" t="s">
         <v>64</v>
       </c>
@@ -1943,6 +2522,9 @@
       <c r="C6" t="s">
         <v>165</v>
       </c>
+      <c r="D6" t="s">
+        <v>440</v>
+      </c>
       <c r="E6" t="s">
         <v>151</v>
       </c>
@@ -1960,6 +2542,9 @@
       <c r="C7" t="s">
         <v>164</v>
       </c>
+      <c r="D7" t="s">
+        <v>441</v>
+      </c>
       <c r="E7" t="s">
         <v>152</v>
       </c>
@@ -1977,6 +2562,9 @@
       <c r="C8" t="s">
         <v>166</v>
       </c>
+      <c r="D8" t="s">
+        <v>442</v>
+      </c>
       <c r="F8" t="s">
         <v>233</v>
       </c>
@@ -1988,6 +2576,9 @@
       <c r="C9" t="s">
         <v>193</v>
       </c>
+      <c r="D9" t="s">
+        <v>443</v>
+      </c>
       <c r="E9" t="s">
         <v>190</v>
       </c>
@@ -2002,6 +2593,9 @@
       <c r="C10" t="s">
         <v>255</v>
       </c>
+      <c r="D10" t="s">
+        <v>444</v>
+      </c>
       <c r="E10" t="s">
         <v>233</v>
       </c>
@@ -2016,6 +2610,9 @@
       <c r="C11" t="s">
         <v>254</v>
       </c>
+      <c r="D11" t="s">
+        <v>445</v>
+      </c>
       <c r="E11" t="s">
         <v>247</v>
       </c>
@@ -2027,6 +2624,9 @@
       <c r="C12" t="s">
         <v>236</v>
       </c>
+      <c r="D12" t="s">
+        <v>446</v>
+      </c>
       <c r="E12" t="s">
         <v>232</v>
       </c>
@@ -2038,6 +2638,9 @@
       <c r="C13" t="s">
         <v>251</v>
       </c>
+      <c r="D13" t="s">
+        <v>447</v>
+      </c>
       <c r="E13" t="s">
         <v>232</v>
       </c>
@@ -2052,6 +2655,9 @@
       <c r="C14" t="s">
         <v>238</v>
       </c>
+      <c r="D14" t="s">
+        <v>448</v>
+      </c>
       <c r="F14" t="s">
         <v>233</v>
       </c>
@@ -2063,6 +2669,9 @@
       <c r="C15" t="s">
         <v>256</v>
       </c>
+      <c r="D15" t="s">
+        <v>449</v>
+      </c>
       <c r="E15" t="s">
         <v>233</v>
       </c>
@@ -2077,6 +2686,9 @@
       <c r="C16" t="s">
         <v>257</v>
       </c>
+      <c r="D16" t="s">
+        <v>450</v>
+      </c>
       <c r="E16" t="s">
         <v>233</v>
       </c>
@@ -2091,6 +2703,9 @@
       <c r="C17" t="s">
         <v>252</v>
       </c>
+      <c r="D17" t="s">
+        <v>451</v>
+      </c>
       <c r="F17" t="s">
         <v>247</v>
       </c>
@@ -2101,6 +2716,9 @@
       </c>
       <c r="C18" t="s">
         <v>253</v>
+      </c>
+      <c r="D18" t="s">
+        <v>452</v>
       </c>
       <c r="E18" t="s">
         <v>247</v>
@@ -2116,7 +2734,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2380,7 +2998,7 @@
         <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -2390,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454B4658-2E66-4A70-8A1A-07C12B18376F}">
-  <dimension ref="A2:D141"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2404,43 +3022,54 @@
     <col min="4" max="4" width="64.1171875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
@@ -2448,21 +3077,21 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
@@ -2470,21 +3099,21 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
@@ -2492,21 +3121,21 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
@@ -2514,21 +3143,21 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
@@ -2536,21 +3165,21 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -2558,21 +3187,21 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.5">
@@ -2580,21 +3209,21 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.5">
@@ -2602,21 +3231,21 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.5">
@@ -2624,10 +3253,10 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.5">
@@ -2635,10 +3264,10 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.5">
@@ -2646,10 +3275,10 @@
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.5">
@@ -2657,21 +3286,21 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.5">
@@ -2679,10 +3308,10 @@
         <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.5">
@@ -2690,10 +3319,10 @@
         <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.5">
@@ -2701,10 +3330,10 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.5">
@@ -2712,10 +3341,10 @@
         <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.5">
@@ -2723,10 +3352,10 @@
         <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.5">
@@ -2734,10 +3363,10 @@
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.5">
@@ -2745,10 +3374,10 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.5">
@@ -2756,21 +3385,21 @@
         <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.5">
@@ -2778,10 +3407,10 @@
         <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.5">
@@ -2789,10 +3418,10 @@
         <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.5">
@@ -2800,10 +3429,10 @@
         <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.5">
@@ -2811,10 +3440,10 @@
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.5">
@@ -2822,10 +3451,10 @@
         <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.5">
@@ -2833,10 +3462,10 @@
         <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.5">
@@ -2844,10 +3473,10 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.5">
@@ -2855,21 +3484,21 @@
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.5">
@@ -2877,10 +3506,10 @@
         <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.5">
@@ -2888,10 +3517,10 @@
         <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.5">
@@ -2899,10 +3528,10 @@
         <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.5">
@@ -2910,10 +3539,10 @@
         <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.5">
@@ -2921,10 +3550,10 @@
         <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.5">
@@ -2932,21 +3561,21 @@
         <v>104</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B50" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.5">
@@ -2954,10 +3583,10 @@
         <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.5">
@@ -2965,21 +3594,21 @@
         <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.5">
@@ -2987,10 +3616,10 @@
         <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.5">
@@ -2998,21 +3627,21 @@
         <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D56" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.5">
@@ -3020,10 +3649,10 @@
         <v>107</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="D57" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.5">
@@ -3031,21 +3660,21 @@
         <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B59" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="C59" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.5">
@@ -3053,7 +3682,10 @@
         <v>194</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>168</v>
+      </c>
+      <c r="D60" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.5">
@@ -3061,7 +3693,10 @@
         <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.5">
@@ -3069,7 +3704,10 @@
         <v>194</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>196</v>
+      </c>
+      <c r="D62" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.5">
@@ -3077,7 +3715,10 @@
         <v>194</v>
       </c>
       <c r="C63" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="D63" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.5">
@@ -3085,330 +3726,777 @@
         <v>194</v>
       </c>
       <c r="C64" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.5">
+        <v>169</v>
+      </c>
+      <c r="D64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B65" t="s">
         <v>194</v>
       </c>
       <c r="C65" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.5">
+        <v>198</v>
+      </c>
+      <c r="D65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B66" t="s">
         <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.5">
+        <v>170</v>
+      </c>
+      <c r="D66" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B67" t="s">
         <v>194</v>
       </c>
       <c r="C67" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.5">
+        <v>110</v>
+      </c>
+      <c r="D67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B68" t="s">
         <v>194</v>
       </c>
       <c r="C68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.5">
+        <v>65</v>
+      </c>
+      <c r="D68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B69" t="s">
         <v>194</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.5">
+        <v>199</v>
+      </c>
+      <c r="D69" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B70" t="s">
         <v>194</v>
       </c>
       <c r="C70" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.5">
+        <v>200</v>
+      </c>
+      <c r="D70" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B71" t="s">
         <v>194</v>
       </c>
       <c r="C71" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.5">
+        <v>116</v>
+      </c>
+      <c r="D71" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B72" t="s">
         <v>194</v>
       </c>
       <c r="C72" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.5">
+        <v>117</v>
+      </c>
+      <c r="D72" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B73" t="s">
         <v>194</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.5">
+        <v>136</v>
+      </c>
+      <c r="D73" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B74" t="s">
         <v>194</v>
       </c>
       <c r="C74" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.5">
+        <v>172</v>
+      </c>
+      <c r="D74" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B75" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.5">
+        <v>42</v>
+      </c>
+      <c r="D75" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B76" t="s">
         <v>184</v>
       </c>
       <c r="C76" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.5">
+        <v>65</v>
+      </c>
+      <c r="D76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B77" t="s">
+        <v>184</v>
+      </c>
       <c r="C77" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.5">
+        <v>201</v>
+      </c>
+      <c r="D77" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B78" t="s">
+        <v>184</v>
+      </c>
       <c r="C78" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.5">
+        <v>202</v>
+      </c>
+      <c r="D78" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B79" t="s">
+        <v>184</v>
+      </c>
       <c r="C79" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+      <c r="D79" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B80" t="s">
+        <v>204</v>
+      </c>
       <c r="C80" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.5">
+        <v>205</v>
+      </c>
+      <c r="D80" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B81" t="s">
         <v>204</v>
       </c>
       <c r="C81" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.5">
+        <v>206</v>
+      </c>
+      <c r="D81" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B82" t="s">
+        <v>204</v>
+      </c>
       <c r="C82" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.5">
+        <v>207</v>
+      </c>
+      <c r="D82" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B83" t="s">
+        <v>204</v>
+      </c>
       <c r="C83" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.5">
+        <v>208</v>
+      </c>
+      <c r="D83" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B84" t="s">
+        <v>204</v>
+      </c>
       <c r="C84" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.5">
+        <v>209</v>
+      </c>
+      <c r="D84" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B85" t="s">
+        <v>204</v>
+      </c>
       <c r="C85" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.5">
+        <v>210</v>
+      </c>
+      <c r="D85" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B86" t="s">
+        <v>204</v>
+      </c>
       <c r="C86" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.5">
+        <v>211</v>
+      </c>
+      <c r="D86" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B87" t="s">
+        <v>212</v>
+      </c>
       <c r="C87" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.5">
+        <v>42</v>
+      </c>
+      <c r="D87" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B88" t="s">
         <v>212</v>
       </c>
       <c r="C88" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.5">
+        <v>43</v>
+      </c>
+      <c r="D88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B89" t="s">
+        <v>212</v>
+      </c>
       <c r="C89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+      <c r="D89" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B90" t="s">
+        <v>212</v>
+      </c>
       <c r="C90" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.5">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B91" t="s">
+        <v>212</v>
+      </c>
       <c r="C91" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.5">
+        <v>215</v>
+      </c>
+      <c r="D91" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B92" t="s">
+        <v>286</v>
+      </c>
       <c r="C92" t="s">
+        <v>287</v>
+      </c>
+      <c r="D92" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B93" t="s">
+        <v>286</v>
+      </c>
+      <c r="C93" t="s">
+        <v>288</v>
+      </c>
+      <c r="D93" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B94" t="s">
+        <v>230</v>
+      </c>
+      <c r="C94" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B95" t="s">
+        <v>230</v>
+      </c>
+      <c r="C95" t="s">
+        <v>84</v>
+      </c>
+      <c r="D95" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B96" t="s">
+        <v>230</v>
+      </c>
+      <c r="C96" t="s">
+        <v>293</v>
+      </c>
+      <c r="D96" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B97" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" t="s">
+        <v>295</v>
+      </c>
+      <c r="D97" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" t="s">
+        <v>297</v>
+      </c>
+      <c r="D98" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B99" t="s">
+        <v>230</v>
+      </c>
+      <c r="C99" t="s">
+        <v>299</v>
+      </c>
+      <c r="D99" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B100" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D100" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B101" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A122" t="s">
+      <c r="D101" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B102" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" t="s">
+        <v>287</v>
+      </c>
+      <c r="D102" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B103" t="s">
+        <v>228</v>
+      </c>
+      <c r="C103" t="s">
+        <v>305</v>
+      </c>
+      <c r="D103" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B104" t="s">
+        <v>228</v>
+      </c>
+      <c r="C104" t="s">
+        <v>306</v>
+      </c>
+      <c r="D104" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B105" t="s">
+        <v>228</v>
+      </c>
+      <c r="C105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D105" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B106" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" t="s">
+        <v>309</v>
+      </c>
+      <c r="D106" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B107" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" t="s">
+        <v>311</v>
+      </c>
+      <c r="D107" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B108" t="s">
+        <v>224</v>
+      </c>
+      <c r="C108" t="s">
+        <v>84</v>
+      </c>
+      <c r="D108" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B109" t="s">
+        <v>224</v>
+      </c>
+      <c r="C109" t="s">
+        <v>314</v>
+      </c>
+      <c r="D109" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B110" t="s">
+        <v>224</v>
+      </c>
+      <c r="C110" t="s">
+        <v>316</v>
+      </c>
+      <c r="D110" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B111" t="s">
+        <v>224</v>
+      </c>
+      <c r="C111" t="s">
+        <v>318</v>
+      </c>
+      <c r="D111" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B112" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112" t="s">
+        <v>320</v>
+      </c>
+      <c r="D112" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B113" t="s">
+        <v>224</v>
+      </c>
+      <c r="C113" t="s">
+        <v>322</v>
+      </c>
+      <c r="D113" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B114" t="s">
+        <v>224</v>
+      </c>
+      <c r="C114" t="s">
+        <v>324</v>
+      </c>
+      <c r="D114" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B115" t="s">
+        <v>224</v>
+      </c>
+      <c r="C115" t="s">
+        <v>326</v>
+      </c>
+      <c r="D115" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B116" t="s">
+        <v>224</v>
+      </c>
+      <c r="C116" t="s">
+        <v>328</v>
+      </c>
+      <c r="D116" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B117" t="s">
+        <v>217</v>
+      </c>
+      <c r="C117" t="s">
+        <v>95</v>
+      </c>
+      <c r="D117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B118" t="s">
+        <v>217</v>
+      </c>
+      <c r="C118" t="s">
+        <v>168</v>
+      </c>
+      <c r="D118" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B119" t="s">
+        <v>217</v>
+      </c>
+      <c r="C119" t="s">
+        <v>84</v>
+      </c>
+      <c r="D119" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B120" t="s">
+        <v>219</v>
+      </c>
+      <c r="C120" t="s">
+        <v>331</v>
+      </c>
+      <c r="D120" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B121" t="s">
+        <v>219</v>
+      </c>
+      <c r="C121" t="s">
+        <v>333</v>
+      </c>
+      <c r="D121" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B122" t="s">
+        <v>219</v>
+      </c>
+      <c r="C122" t="s">
+        <v>336</v>
+      </c>
+      <c r="D122" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B123" t="s">
+        <v>219</v>
+      </c>
+      <c r="C123" t="s">
+        <v>338</v>
+      </c>
+      <c r="D123" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B124" t="s">
+        <v>219</v>
+      </c>
+      <c r="C124" t="s">
+        <v>215</v>
+      </c>
+      <c r="D124" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B125" t="s">
+        <v>219</v>
+      </c>
+      <c r="C125" t="s">
+        <v>341</v>
+      </c>
+      <c r="D125" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B126" t="s">
+        <v>219</v>
+      </c>
+      <c r="C126" t="s">
+        <v>342</v>
+      </c>
+      <c r="D126" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B127" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" t="s">
+        <v>343</v>
+      </c>
+      <c r="D127" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B128" t="s">
+        <v>219</v>
+      </c>
+      <c r="C128" t="s">
+        <v>344</v>
+      </c>
+      <c r="D128" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B129" t="s">
+        <v>219</v>
+      </c>
+      <c r="C129" t="s">
+        <v>345</v>
+      </c>
+      <c r="D129" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B130" t="s">
+        <v>219</v>
+      </c>
+      <c r="C130" t="s">
+        <v>346</v>
+      </c>
+      <c r="D130" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B131" t="s">
+        <v>219</v>
+      </c>
+      <c r="C131" t="s">
+        <v>347</v>
+      </c>
+      <c r="D131" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B132" t="s">
+        <v>219</v>
+      </c>
+      <c r="C132" t="s">
+        <v>348</v>
+      </c>
+      <c r="D132" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B133" t="s">
+        <v>219</v>
+      </c>
+      <c r="C133" t="s">
+        <v>84</v>
+      </c>
+      <c r="D133" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A134" t="s">
         <v>57</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B134" t="s">
         <v>56</v>
-      </c>
-      <c r="C122" t="s">
-        <v>84</v>
-      </c>
-      <c r="D122" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B123" t="s">
-        <v>56</v>
-      </c>
-      <c r="C123" t="s">
-        <v>65</v>
-      </c>
-      <c r="D123" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B124" t="s">
-        <v>56</v>
-      </c>
-      <c r="C124" t="s">
-        <v>87</v>
-      </c>
-      <c r="D124" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B125" t="s">
-        <v>56</v>
-      </c>
-      <c r="C125" t="s">
-        <v>89</v>
-      </c>
-      <c r="D125" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B126" t="s">
-        <v>56</v>
-      </c>
-      <c r="C126" t="s">
-        <v>91</v>
-      </c>
-      <c r="D126" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B127" t="s">
-        <v>56</v>
-      </c>
-      <c r="C127" t="s">
-        <v>92</v>
-      </c>
-      <c r="D127" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B128" t="s">
-        <v>56</v>
-      </c>
-      <c r="C128" t="s">
-        <v>95</v>
-      </c>
-      <c r="D128" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B129" t="s">
-        <v>83</v>
-      </c>
-      <c r="C129" t="s">
-        <v>84</v>
-      </c>
-      <c r="D129" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B130" t="s">
-        <v>83</v>
-      </c>
-      <c r="C130" t="s">
-        <v>65</v>
-      </c>
-      <c r="D130" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B131" t="s">
-        <v>83</v>
-      </c>
-      <c r="C131" t="s">
-        <v>97</v>
-      </c>
-      <c r="D131" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B132" t="s">
-        <v>83</v>
-      </c>
-      <c r="C132" t="s">
-        <v>99</v>
-      </c>
-      <c r="D132" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B133" t="s">
-        <v>171</v>
-      </c>
-      <c r="C133" t="s">
-        <v>168</v>
-      </c>
-      <c r="D133" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B134" t="s">
-        <v>171</v>
       </c>
       <c r="C134" t="s">
         <v>84</v>
@@ -3417,9 +4505,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B135" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="C135" t="s">
         <v>65</v>
@@ -3428,70 +4516,818 @@
         <v>86</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B136" t="s">
+        <v>56</v>
+      </c>
+      <c r="C136" t="s">
+        <v>87</v>
+      </c>
+      <c r="D136" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B137" t="s">
+        <v>56</v>
+      </c>
+      <c r="C137" t="s">
+        <v>89</v>
+      </c>
+      <c r="D137" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B138" t="s">
+        <v>56</v>
+      </c>
+      <c r="C138" t="s">
+        <v>91</v>
+      </c>
+      <c r="D138" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B139" t="s">
+        <v>56</v>
+      </c>
+      <c r="C139" t="s">
+        <v>92</v>
+      </c>
+      <c r="D139" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B140" t="s">
+        <v>56</v>
+      </c>
+      <c r="C140" t="s">
+        <v>95</v>
+      </c>
+      <c r="D140" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+      <c r="C141" t="s">
+        <v>84</v>
+      </c>
+      <c r="D141" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B142" t="s">
+        <v>83</v>
+      </c>
+      <c r="C142" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B143" t="s">
+        <v>83</v>
+      </c>
+      <c r="C143" t="s">
+        <v>97</v>
+      </c>
+      <c r="D143" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="B144" t="s">
+        <v>83</v>
+      </c>
+      <c r="C144" t="s">
+        <v>99</v>
+      </c>
+      <c r="D144" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B145" t="s">
         <v>171</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C145" t="s">
+        <v>168</v>
+      </c>
+      <c r="D145" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B146" t="s">
+        <v>171</v>
+      </c>
+      <c r="C146" t="s">
+        <v>84</v>
+      </c>
+      <c r="D146" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B147" t="s">
+        <v>171</v>
+      </c>
+      <c r="C147" t="s">
+        <v>65</v>
+      </c>
+      <c r="D147" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B148" t="s">
+        <v>171</v>
+      </c>
+      <c r="C148" t="s">
         <v>169</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D148" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B137" t="s">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B149" t="s">
         <v>171</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C149" t="s">
         <v>170</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D149" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B138" t="s">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B150" t="s">
         <v>171</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C150" t="s">
         <v>172</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D150" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B139" t="s">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B151" t="s">
         <v>171</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C151" t="s">
         <v>173</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D151" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B140" t="s">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B152" t="s">
         <v>171</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C152" t="s">
         <v>174</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D152" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B141" t="s">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B153" t="s">
         <v>171</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C153" t="s">
         <v>175</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D153" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B154" t="s">
+        <v>166</v>
+      </c>
+      <c r="C154" t="s">
+        <v>168</v>
+      </c>
+      <c r="D154" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B155" t="s">
+        <v>166</v>
+      </c>
+      <c r="C155" t="s">
+        <v>84</v>
+      </c>
+      <c r="D155" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B156" t="s">
+        <v>166</v>
+      </c>
+      <c r="C156" t="s">
+        <v>358</v>
+      </c>
+      <c r="D156" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B157" t="s">
+        <v>166</v>
+      </c>
+      <c r="C157" t="s">
+        <v>360</v>
+      </c>
+      <c r="D157" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B158" t="s">
+        <v>166</v>
+      </c>
+      <c r="C158" t="s">
+        <v>362</v>
+      </c>
+      <c r="D158" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B159" t="s">
+        <v>166</v>
+      </c>
+      <c r="C159" t="s">
+        <v>364</v>
+      </c>
+      <c r="D159" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B160" t="s">
+        <v>166</v>
+      </c>
+      <c r="C160" t="s">
+        <v>65</v>
+      </c>
+      <c r="D160" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B161" t="s">
+        <v>166</v>
+      </c>
+      <c r="C161" t="s">
+        <v>367</v>
+      </c>
+      <c r="D161" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B162" t="s">
+        <v>166</v>
+      </c>
+      <c r="C162" t="s">
+        <v>369</v>
+      </c>
+      <c r="D162" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B163" t="s">
+        <v>166</v>
+      </c>
+      <c r="C163" t="s">
+        <v>370</v>
+      </c>
+      <c r="D163" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B164" t="s">
+        <v>166</v>
+      </c>
+      <c r="C164" t="s">
+        <v>373</v>
+      </c>
+      <c r="D164" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B165" t="s">
+        <v>166</v>
+      </c>
+      <c r="C165" t="s">
+        <v>333</v>
+      </c>
+      <c r="D165" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B166" t="s">
+        <v>166</v>
+      </c>
+      <c r="C166" t="s">
+        <v>375</v>
+      </c>
+      <c r="D166" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B167" t="s">
+        <v>166</v>
+      </c>
+      <c r="C167" t="s">
+        <v>377</v>
+      </c>
+      <c r="D167" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B168" t="s">
+        <v>166</v>
+      </c>
+      <c r="C168" t="s">
+        <v>379</v>
+      </c>
+      <c r="D168" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B169" t="s">
+        <v>254</v>
+      </c>
+      <c r="C169" t="s">
+        <v>84</v>
+      </c>
+      <c r="D169" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B170" t="s">
+        <v>254</v>
+      </c>
+      <c r="C170" t="s">
+        <v>65</v>
+      </c>
+      <c r="D170" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B171" t="s">
+        <v>254</v>
+      </c>
+      <c r="C171" t="s">
+        <v>333</v>
+      </c>
+      <c r="D171" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B172" t="s">
+        <v>254</v>
+      </c>
+      <c r="C172" t="s">
+        <v>383</v>
+      </c>
+      <c r="D172" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B173" t="s">
+        <v>254</v>
+      </c>
+      <c r="C173" t="s">
+        <v>385</v>
+      </c>
+      <c r="D173" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B174" t="s">
+        <v>254</v>
+      </c>
+      <c r="C174" t="s">
+        <v>387</v>
+      </c>
+      <c r="D174" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B175" t="s">
+        <v>193</v>
+      </c>
+      <c r="C175" t="s">
+        <v>84</v>
+      </c>
+      <c r="D175" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B176" t="s">
+        <v>193</v>
+      </c>
+      <c r="C176" t="s">
+        <v>42</v>
+      </c>
+      <c r="D176" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B177" t="s">
+        <v>193</v>
+      </c>
+      <c r="C177" t="s">
+        <v>65</v>
+      </c>
+      <c r="D177" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B178" t="s">
+        <v>193</v>
+      </c>
+      <c r="C178" t="s">
+        <v>172</v>
+      </c>
+      <c r="D178" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B179" t="s">
+        <v>256</v>
+      </c>
+      <c r="C179" t="s">
+        <v>84</v>
+      </c>
+      <c r="D179" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B180" t="s">
+        <v>256</v>
+      </c>
+      <c r="C180" t="s">
+        <v>392</v>
+      </c>
+      <c r="D180" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B181" t="s">
+        <v>256</v>
+      </c>
+      <c r="C181" t="s">
+        <v>393</v>
+      </c>
+      <c r="D181" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B182" t="s">
+        <v>257</v>
+      </c>
+      <c r="C182" t="s">
+        <v>393</v>
+      </c>
+      <c r="D182" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B183" t="s">
+        <v>251</v>
+      </c>
+      <c r="C183" t="s">
+        <v>84</v>
+      </c>
+      <c r="D183" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B184" t="s">
+        <v>251</v>
+      </c>
+      <c r="C184" t="s">
+        <v>396</v>
+      </c>
+      <c r="D184" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B185" t="s">
+        <v>251</v>
+      </c>
+      <c r="C185" t="s">
+        <v>398</v>
+      </c>
+      <c r="D185" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B186" t="s">
+        <v>251</v>
+      </c>
+      <c r="C186" t="s">
+        <v>400</v>
+      </c>
+      <c r="D186" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B187" t="s">
+        <v>251</v>
+      </c>
+      <c r="C187" t="s">
+        <v>402</v>
+      </c>
+      <c r="D187" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B188" t="s">
+        <v>251</v>
+      </c>
+      <c r="C188" t="s">
+        <v>405</v>
+      </c>
+      <c r="D188" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B189" t="s">
+        <v>252</v>
+      </c>
+      <c r="C189" t="s">
+        <v>84</v>
+      </c>
+      <c r="D189" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B190" t="s">
+        <v>252</v>
+      </c>
+      <c r="C190" t="s">
+        <v>345</v>
+      </c>
+      <c r="D190" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B191" t="s">
+        <v>252</v>
+      </c>
+      <c r="C191" t="s">
+        <v>346</v>
+      </c>
+      <c r="D191" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B192" t="s">
+        <v>252</v>
+      </c>
+      <c r="C192" t="s">
+        <v>347</v>
+      </c>
+      <c r="D192" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B193" t="s">
+        <v>252</v>
+      </c>
+      <c r="C193" t="s">
+        <v>196</v>
+      </c>
+      <c r="D193" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B194" t="s">
+        <v>252</v>
+      </c>
+      <c r="C194" t="s">
+        <v>411</v>
+      </c>
+      <c r="D194" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B195" t="s">
+        <v>252</v>
+      </c>
+      <c r="C195" t="s">
+        <v>410</v>
+      </c>
+      <c r="D195" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B196" t="s">
+        <v>252</v>
+      </c>
+      <c r="C196" t="s">
+        <v>413</v>
+      </c>
+      <c r="D196" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B197" t="s">
+        <v>252</v>
+      </c>
+      <c r="C197" t="s">
+        <v>415</v>
+      </c>
+      <c r="D197" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B198" t="s">
+        <v>252</v>
+      </c>
+      <c r="C198" t="s">
+        <v>417</v>
+      </c>
+      <c r="D198" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B199" t="s">
+        <v>252</v>
+      </c>
+      <c r="C199" t="s">
+        <v>419</v>
+      </c>
+      <c r="D199" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B200" t="s">
+        <v>252</v>
+      </c>
+      <c r="C200" t="s">
+        <v>421</v>
+      </c>
+      <c r="D200" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B201" t="s">
+        <v>252</v>
+      </c>
+      <c r="C201" t="s">
+        <v>423</v>
+      </c>
+      <c r="D201" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B202" t="s">
+        <v>252</v>
+      </c>
+      <c r="C202" t="s">
+        <v>425</v>
+      </c>
+      <c r="D202" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B203" t="s">
+        <v>252</v>
+      </c>
+      <c r="C203" t="s">
+        <v>427</v>
+      </c>
+      <c r="D203" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B204" t="s">
+        <v>252</v>
+      </c>
+      <c r="C204" t="s">
+        <v>429</v>
+      </c>
+      <c r="D204" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B205" t="s">
+        <v>252</v>
+      </c>
+      <c r="C205" t="s">
+        <v>431</v>
+      </c>
+      <c r="D205" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B206" t="s">
+        <v>253</v>
+      </c>
+      <c r="C206" t="s">
+        <v>84</v>
+      </c>
+      <c r="D206" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B207" t="s">
+        <v>253</v>
+      </c>
+      <c r="C207" t="s">
+        <v>392</v>
+      </c>
+      <c r="D207" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B208" t="s">
+        <v>253</v>
+      </c>
+      <c r="C208" t="s">
+        <v>393</v>
+      </c>
+      <c r="D208" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B209" t="s">
+        <v>253</v>
+      </c>
+      <c r="C209" t="s">
+        <v>435</v>
+      </c>
+      <c r="D209" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>